<commit_message>
feature engineering from timestamp
</commit_message>
<xml_diff>
--- a/Data/meter_id/daftar_gedung_sudah_total.xlsx
+++ b/Data/meter_id/daftar_gedung_sudah_total.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFolder\Git\TA_SpatioTemporal\Data\meter_id\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C50E08-92C7-4619-AFE6-2E9DBF48DC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BF0069-B609-4929-8051-73A87AA814DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="117">
   <si>
     <t>No</t>
   </si>
@@ -318,9 +318,6 @@
     <t>-6.891765358434122, 107.60900820240957</t>
   </si>
   <si>
-    <t xml:space="preserve">SBM </t>
-  </si>
-  <si>
     <t>SBM MDP Total</t>
   </si>
   <si>
@@ -406,6 +403,12 @@
   </si>
   <si>
     <t>LABTEK IV Geologi</t>
+  </si>
+  <si>
+    <t>Lift</t>
+  </si>
+  <si>
+    <t>SBM</t>
   </si>
 </sst>
 </file>
@@ -853,8 +856,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D339290F-3E77-4B5F-9417-5D90519CDC41}" name="gedung_terpakai" displayName="gedung_terpakai" ref="A1:F71" headerRowDxfId="13" dataDxfId="11" totalsRowDxfId="9" headerRowBorderDxfId="12" tableBorderDxfId="10">
-  <autoFilter ref="A1:F71" xr:uid="{D339290F-3E77-4B5F-9417-5D90519CDC41}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D339290F-3E77-4B5F-9417-5D90519CDC41}" name="gedung_terpakai" displayName="gedung_terpakai" ref="A1:F72" headerRowDxfId="13" dataDxfId="11" totalsRowDxfId="9" headerRowBorderDxfId="12" tableBorderDxfId="10">
+  <autoFilter ref="A1:F72" xr:uid="{D339290F-3E77-4B5F-9417-5D90519CDC41}"/>
   <tableColumns count="6">
     <tableColumn id="3" xr3:uid="{6FA353D7-1CAA-4D68-BF07-D735B94C59A4}" name="No" dataDxfId="8">
       <calculatedColumnFormula array="1">ROW() - ROW(gedung_terpakai[#Headers])</calculatedColumnFormula>
@@ -1132,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4332F93-D836-4DD4-8134-A919422D62FC}">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1227,7 +1230,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1239,14 +1242,14 @@
         <v>122141</v>
       </c>
       <c r="C5" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>102</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>103</v>
       </c>
       <c r="E5" s="19"/>
       <c r="F5" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1258,10 +1261,10 @@
         <v>122131</v>
       </c>
       <c r="C6" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>102</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>103</v>
       </c>
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
@@ -1275,10 +1278,10 @@
         <v>122121</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
@@ -1292,10 +1295,10 @@
         <v>122111</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
@@ -1525,7 +1528,7 @@
         <v>145001</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>7</v>
@@ -1546,7 +1549,7 @@
         <v>145002</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>7</v>
@@ -1563,7 +1566,7 @@
         <v>130001</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>7</v>
@@ -1572,7 +1575,7 @@
         <v>8</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1584,7 +1587,7 @@
         <v>130002</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>7</v>
@@ -1610,7 +1613,7 @@
         <v>9</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1711,7 +1714,7 @@
         <v>13</v>
       </c>
       <c r="F30" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1963,7 +1966,7 @@
         <v>104001</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>49</v>
@@ -1984,7 +1987,7 @@
         <v>104002</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>51</v>
@@ -2005,7 +2008,7 @@
         <v>109111</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>53</v>
@@ -2026,7 +2029,7 @@
         <v>109011</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D46" s="20" t="s">
         <v>55</v>
@@ -2045,7 +2048,7 @@
         <v>109001</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>57</v>
@@ -2338,16 +2341,16 @@
         <v>163</v>
       </c>
       <c r="C62" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D62" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="E62" s="4">
         <v>35</v>
       </c>
       <c r="F62" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2356,40 +2359,36 @@
         <v>62</v>
       </c>
       <c r="B63" s="4">
-        <v>118001</v>
+        <v>118002</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E63" s="4">
-        <v>36</v>
-      </c>
-      <c r="F63" s="15" t="s">
-        <v>90</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="7" cm="1">
+      <c r="A64" s="4" cm="1">
         <f t="array" ref="A64">ROW() - ROW(gedung_terpakai[#Headers])</f>
         <v>63</v>
       </c>
-      <c r="B64" s="8">
-        <v>101011</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E64" s="7">
-        <v>37</v>
-      </c>
-      <c r="F64" s="8" t="s">
-        <v>93</v>
+      <c r="B64" s="4">
+        <v>118001</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E64" s="4">
+        <v>36</v>
+      </c>
+      <c r="F64" s="15" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -2398,16 +2397,20 @@
         <v>64</v>
       </c>
       <c r="B65" s="8">
-        <v>101010</v>
+        <v>101011</v>
       </c>
       <c r="C65" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D65" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D65" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E65" s="7"/>
-      <c r="F65" s="7"/>
+      <c r="E65" s="7">
+        <v>37</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="7" cm="1">
@@ -2415,13 +2418,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="8">
-        <v>101012</v>
+        <v>101010</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
@@ -2432,13 +2435,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="8">
-        <v>101013</v>
+        <v>101012</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
@@ -2449,13 +2452,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="8">
-        <v>101021</v>
+        <v>101013</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
@@ -2466,13 +2469,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="8">
-        <v>101022</v>
+        <v>101021</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
@@ -2483,13 +2486,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="8">
-        <v>101023</v>
+        <v>101022</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
@@ -2500,16 +2503,33 @@
         <v>70</v>
       </c>
       <c r="B71" s="8">
-        <v>101201</v>
+        <v>101023</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="7" cm="1">
+        <f t="array" ref="A72">ROW() - ROW(gedung_terpakai[#Headers])</f>
+        <v>71</v>
+      </c>
+      <c r="B72" s="8">
+        <v>101201</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>